<commit_message>
Update of analyses for article
</commit_message>
<xml_diff>
--- a/docs/sample for speechacts.xlsx
+++ b/docs/sample for speechacts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FrankVerhoef/Programming/PEX/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FrankVerhoef/Programming/PEX/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA6979F-93D0-FC47-9568-A7175169266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F400812-42C4-D844-AF2B-63AE05A847A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="32280" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -18041,126 +18041,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB2FE99E-E1B9-3549-9A26-F30014C8B335}" name="Draaitabel3" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A71:F75" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="34">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0" sortType="descending">
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="20"/>
-  </colFields>
-  <colItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="6" hier="-1"/>
-  </pageFields>
-  <dataFields count="3">
-    <dataField name="Aantal van convai_id" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Gemiddelde van len_t_split" fld="12" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
-    <dataField name="Gemiddelde van len_p_split" fld="11" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C05A385C-CABF-FA40-B20D-69903B501AB1}" name="Draaitabel2" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C05A385C-CABF-FA40-B20D-69903B501AB1}" name="Draaitabel2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A24:F60" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="34">
     <pivotField showAll="0"/>
@@ -18383,8 +18264,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Draaitabel1" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Draaitabel1" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:V11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="34">
     <pivotField showAll="0"/>
@@ -18564,8 +18445,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5E129C9-636C-9C48-83D6-731E70DA8826}" name="Draaitabel4" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5E129C9-636C-9C48-83D6-731E70DA8826}" name="Draaitabel4" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A82:F86" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="34">
     <pivotField showAll="0"/>
@@ -18670,6 +18551,125 @@
     <dataField name="Aantal van convai_id" fld="3" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Gemiddelde van len_p" fld="13" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
     <dataField name="Gemiddelde van len_t" fld="14" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB2FE99E-E1B9-3549-9A26-F30014C8B335}" name="Draaitabel3" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A71:F75" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="34">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" sortType="descending">
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="20"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="6" hier="-1"/>
+  </pageFields>
+  <dataFields count="3">
+    <dataField name="Aantal van convai_id" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Gemiddelde van len_t_split" fld="12" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Gemiddelde van len_p_split" fld="11" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -19982,14 +19982,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AJ1048345"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="V258" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB258" sqref="AB258"/>
+      <selection pane="bottomRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20117,7 +20116,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -20231,7 +20230,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -20345,7 +20344,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -20459,7 +20458,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -20573,7 +20572,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -20772,7 +20771,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -20948,7 +20947,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -21062,7 +21061,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -21147,7 +21146,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -21261,7 +21260,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -21346,7 +21345,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -21437,7 +21436,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -21551,7 +21550,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -21665,7 +21664,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -21750,7 +21749,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -21835,7 +21834,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" ht="102" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>1</v>
       </c>
@@ -21949,7 +21948,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -22034,7 +22033,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>1</v>
       </c>
@@ -22233,7 +22232,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -22324,7 +22323,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -22506,7 +22505,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -22597,7 +22596,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>1</v>
       </c>
@@ -22682,7 +22681,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -22773,7 +22772,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>1</v>
       </c>
@@ -22858,7 +22857,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>1</v>
       </c>
@@ -22943,7 +22942,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>1</v>
       </c>
@@ -23034,7 +23033,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>1</v>
       </c>
@@ -23119,7 +23118,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>1</v>
       </c>
@@ -23324,7 +23323,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>1</v>
       </c>
@@ -23415,7 +23414,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>1</v>
       </c>
@@ -23500,7 +23499,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="37" spans="1:36" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:36" ht="85" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>1</v>
       </c>
@@ -23705,7 +23704,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="39" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>1</v>
       </c>
@@ -23819,7 +23818,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>1</v>
       </c>
@@ -23933,7 +23932,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>1</v>
       </c>
@@ -24024,7 +24023,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>1</v>
       </c>
@@ -24229,7 +24228,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>1</v>
       </c>
@@ -24343,7 +24342,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="45" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>1</v>
       </c>
@@ -24457,7 +24456,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="46" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>1</v>
       </c>
@@ -24571,7 +24570,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="47" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>1</v>
       </c>
@@ -24662,7 +24661,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>1</v>
       </c>
@@ -24776,7 +24775,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>1</v>
       </c>
@@ -24867,7 +24866,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>1</v>
       </c>
@@ -25043,7 +25042,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>1</v>
       </c>
@@ -25157,7 +25156,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>1</v>
       </c>
@@ -25424,7 +25423,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>1</v>
       </c>
@@ -25515,7 +25514,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>1</v>
       </c>
@@ -25629,7 +25628,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>1</v>
       </c>
@@ -25743,7 +25742,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>1</v>
       </c>
@@ -25834,7 +25833,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="60" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>1</v>
       </c>
@@ -25948,7 +25947,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="61" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>1</v>
       </c>
@@ -26033,7 +26032,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="62" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>1</v>
       </c>
@@ -26124,7 +26123,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="63" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>1</v>
       </c>
@@ -26215,7 +26214,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="64" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>1</v>
       </c>
@@ -26300,7 +26299,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="65" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>1</v>
       </c>
@@ -26414,7 +26413,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="66" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>1</v>
       </c>
@@ -26499,7 +26498,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="67" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>1</v>
       </c>
@@ -26584,7 +26583,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="68" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>1</v>
       </c>
@@ -26675,7 +26674,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="69" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>1</v>
       </c>
@@ -26874,7 +26873,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="71" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>1</v>
       </c>
@@ -27739,7 +27738,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="80" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>2</v>
       </c>
@@ -28097,7 +28096,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="84" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>2</v>
       </c>
@@ -28381,7 +28380,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="87" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>2</v>
       </c>
@@ -29495,7 +29494,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="99" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>2</v>
       </c>
@@ -29955,7 +29954,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="104" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>2</v>
       </c>
@@ -30222,7 +30221,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="107" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>2</v>
       </c>
@@ -30665,7 +30664,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="112" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>2</v>
       </c>
@@ -31319,7 +31318,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="119" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>2</v>
       </c>
@@ -31433,7 +31432,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="120" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>2</v>
       </c>
@@ -31609,7 +31608,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="122" spans="1:36" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:36" ht="102" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>2</v>
       </c>
@@ -31723,7 +31722,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="123" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>2</v>
       </c>
@@ -31808,7 +31807,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="124" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>2</v>
       </c>
@@ -31893,7 +31892,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="125" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>2</v>
       </c>
@@ -32098,7 +32097,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="127" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>2</v>
       </c>
@@ -32394,7 +32393,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="130" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>2</v>
       </c>
@@ -33895,7 +33894,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="146" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>2</v>
       </c>
@@ -34611,7 +34610,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="154" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>2</v>
       </c>
@@ -34793,7 +34792,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="156" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>2</v>
       </c>
@@ -34907,7 +34906,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="157" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>2</v>
       </c>
@@ -34992,7 +34991,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="158" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>2</v>
       </c>
@@ -35259,7 +35258,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="161" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>2</v>
       </c>
@@ -35605,7 +35604,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="165" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>2</v>
       </c>
@@ -36129,7 +36128,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="170" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>3</v>
       </c>
@@ -36311,7 +36310,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="172" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>3</v>
       </c>
@@ -37330,7 +37329,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="182" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>3</v>
       </c>
@@ -37535,7 +37534,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="184" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>3</v>
       </c>
@@ -37740,7 +37739,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="186" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>3</v>
       </c>
@@ -37916,7 +37915,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="188" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>3</v>
       </c>
@@ -38200,7 +38199,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="191" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>3</v>
       </c>
@@ -38467,7 +38466,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="194" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>3</v>
       </c>
@@ -39355,7 +39354,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="203" spans="1:36" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:36" ht="136" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
         <v>3</v>
       </c>
@@ -39440,7 +39439,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="204" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
         <v>3</v>
       </c>
@@ -39622,7 +39621,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="206" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
         <v>3</v>
       </c>
@@ -39964,7 +39963,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="209" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
         <v>3</v>
       </c>
@@ -40612,7 +40611,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="216" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
         <v>3</v>
       </c>
@@ -40811,7 +40810,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="218" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
         <v>3</v>
       </c>
@@ -41277,7 +41276,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="223" spans="1:36" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
         <v>3</v>
       </c>
@@ -41362,7 +41361,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="224" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
         <v>3</v>
       </c>
@@ -41805,7 +41804,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="229" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
         <v>3</v>
       </c>
@@ -42414,7 +42413,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="235" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
         <v>3</v>
       </c>
@@ -43364,7 +43363,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="245" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
         <v>3</v>
       </c>
@@ -44712,7 +44711,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="259" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A259" s="2">
         <v>4</v>
       </c>
@@ -45588,7 +45587,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="268" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A268" s="2">
         <v>4</v>
       </c>
@@ -47617,7 +47616,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="290" spans="1:36" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A290" s="2">
         <v>4</v>
       </c>
@@ -47708,7 +47707,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="291" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A291" s="2">
         <v>4</v>
       </c>
@@ -47975,7 +47974,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="294" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A294" s="2">
         <v>4</v>
       </c>
@@ -48066,7 +48065,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="295" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A295" s="2">
         <v>4</v>
       </c>
@@ -49062,7 +49061,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="305" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A305" s="2">
         <v>4</v>
       </c>
@@ -49153,7 +49152,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="306" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A306" s="2">
         <v>4</v>
       </c>
@@ -49329,7 +49328,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="308" spans="1:36" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:36" ht="102" x14ac:dyDescent="0.2">
       <c r="A308" s="2">
         <v>4</v>
       </c>
@@ -50273,7 +50272,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="318" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A318" s="2">
         <v>4</v>
       </c>
@@ -50449,7 +50448,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="320" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A320" s="2">
         <v>4</v>
       </c>
@@ -51626,7 +51625,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="332" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A332" s="2">
         <v>4</v>
       </c>
@@ -52394,7 +52393,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="340" spans="1:36" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:36" ht="34" x14ac:dyDescent="0.2">
       <c r="A340" s="2">
         <v>4</v>
       </c>
@@ -53124,231 +53123,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AJ345" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="27">
-      <filters>
-        <filter val="A-EE"/>
-        <filter val="A-EQ"/>
-        <filter val="A-RE"/>
-        <filter val="A-REE"/>
-        <filter val="A-REER"/>
-        <filter val="A-ROQE"/>
-        <filter val="A-SE"/>
-        <filter val="AAE-RES"/>
-        <filter val="AAEQ-AEEA"/>
-        <filter val="AE-EEQQ"/>
-        <filter val="AE-EQ"/>
-        <filter val="AE-PEE"/>
-        <filter val="AE-REE"/>
-        <filter val="AE-REPR"/>
-        <filter val="AE-REQ"/>
-        <filter val="AE-RQ"/>
-        <filter val="AE-RQEESSR"/>
-        <filter val="AE-SEE"/>
-        <filter val="AE-SQ"/>
-        <filter val="AEAQ-AQ"/>
-        <filter val="AEE-EEE"/>
-        <filter val="AEE-EP"/>
-        <filter val="AEE-ERSS"/>
-        <filter val="AEE-ESS"/>
-        <filter val="AEE-Q"/>
-        <filter val="AEE-REEEEEEE"/>
-        <filter val="AEE-REEQ"/>
-        <filter val="AEE-RSP"/>
-        <filter val="AEE-SOQ"/>
-        <filter val="AEE-SSSEEQQ"/>
-        <filter val="AEEE-ESSER"/>
-        <filter val="AEEE-QE"/>
-        <filter val="AEEE-REQ"/>
-        <filter val="AEEEEE-ROPQ"/>
-        <filter val="AEEEQE-AQQ"/>
-        <filter val="AEEOSR-OEOE"/>
-        <filter val="AEEPE-EEPQ"/>
-        <filter val="AEEQ-EEAE"/>
-        <filter val="AEEQ-EEEEAE"/>
-        <filter val="AEEQ-S"/>
-        <filter val="AEEQP-RSEQ"/>
-        <filter val="AEES-OP"/>
-        <filter val="AEO-ROE"/>
-        <filter val="AEP-REQ"/>
-        <filter val="AEPE-RAPP"/>
-        <filter val="AEQ-AEEEQ"/>
-        <filter val="AEQS-ESESQ"/>
-        <filter val="AERE-REP"/>
-        <filter val="AES-EEQ"/>
-        <filter val="AES-EQ"/>
-        <filter val="AESEPE-RSSQ"/>
-        <filter val="AESEQ-RS"/>
-        <filter val="AESQE-SSOEEEE"/>
-        <filter val="AO-E"/>
-        <filter val="AO-QEQ"/>
-        <filter val="AOE-AEEEE"/>
-        <filter val="AOSP-ROEEE"/>
-        <filter val="APE-AQ"/>
-        <filter val="APE-ERRQS"/>
-        <filter val="APEQ-QOS"/>
-        <filter val="AQ-AEP"/>
-        <filter val="AQ-ASE"/>
-        <filter val="AQ-SE"/>
-        <filter val="AQQQQEEE-OQ"/>
-        <filter val="ARS-ESEQ"/>
-        <filter val="AS-OEEEE"/>
-        <filter val="AS-OEQ"/>
-        <filter val="AS-QE"/>
-        <filter val="AS-REEQ"/>
-        <filter val="AS-SEEE"/>
-        <filter val="AS-SEEEEPE"/>
-        <filter val="ASE-EQ"/>
-        <filter val="ASE-OEOOOQ"/>
-        <filter val="ASE-OSQ"/>
-        <filter val="ASE-REEQ"/>
-        <filter val="ASE-ROE"/>
-        <filter val="ASEQ-SSSQ"/>
-        <filter val="ASQ-AAE"/>
-        <filter val="ASQO-OEO"/>
-        <filter val="ASSE-QQ"/>
-        <filter val="ASSESR-ESESSQ"/>
-        <filter val="ASSESS-SEQ"/>
-        <filter val="E-E"/>
-        <filter val="E-EE"/>
-        <filter val="E-EQ"/>
-        <filter val="E-EQE"/>
-        <filter val="E-ERQ"/>
-        <filter val="E-RE"/>
-        <filter val="E-RQ"/>
-        <filter val="E-RQE"/>
-        <filter val="EE-E"/>
-        <filter val="EE-EQQ"/>
-        <filter val="EE-OEESRQ"/>
-        <filter val="EE-RS"/>
-        <filter val="EEE-EO"/>
-        <filter val="EEE-REQ"/>
-        <filter val="EEEE-EOEQ"/>
-        <filter val="EEEE-REE"/>
-        <filter val="EEEQE-AEQ"/>
-        <filter val="EEO-EEO"/>
-        <filter val="EEO-RRRQ"/>
-        <filter val="EEP-QPA"/>
-        <filter val="EEPQ-EAAE"/>
-        <filter val="EEQ-AO"/>
-        <filter val="EERQ-AQQR"/>
-        <filter val="EES-RQ"/>
-        <filter val="EES-SEE"/>
-        <filter val="EESQ-AAEEEE"/>
-        <filter val="EO-E"/>
-        <filter val="EOA-EQQ"/>
-        <filter val="EOO-REQ"/>
-        <filter val="EPP-A"/>
-        <filter val="EQSE-ASQ"/>
-        <filter val="ES-EOPS"/>
-        <filter val="ES-EQ"/>
-        <filter val="ES-REE"/>
-        <filter val="ES-RO"/>
-        <filter val="ESE-EEQ"/>
-        <filter val="ESE-OQ"/>
-        <filter val="ESEE-SOEOQQ"/>
-        <filter val="ESSP-QEE"/>
-        <filter val="O-RE"/>
-        <filter val="OEE-ROEEQ"/>
-        <filter val="OEQS-ROS"/>
-        <filter val="OOE-SES"/>
-        <filter val="OP-RPSEQ"/>
-        <filter val="OS-RQE"/>
-        <filter val="OSOE-ES"/>
-        <filter val="P-AEQP"/>
-        <filter val="PAP-RPPE"/>
-        <filter val="PE-P"/>
-        <filter val="PE-RPEQ"/>
-        <filter val="PE-RS"/>
-        <filter val="Q-AAEEQ"/>
-        <filter val="Q-AE"/>
-        <filter val="Q-AEQ"/>
-        <filter val="Q-QERP"/>
-        <filter val="QE-A"/>
-        <filter val="QE-AR"/>
-        <filter val="QQES-ASERAEEP"/>
-        <filter val="QQO-AEEE"/>
-        <filter val="QQPPE-ES"/>
-        <filter val="QREQOEEPE-RPERQ"/>
-        <filter val="QS-AEEPO"/>
-        <filter val="QSE-EE"/>
-        <filter val="RAOESS-RSP"/>
-        <filter val="RE-EEO"/>
-        <filter val="RE-EEQ"/>
-        <filter val="REE-EEQ"/>
-        <filter val="REE-RSS"/>
-        <filter val="REEE-EEEE"/>
-        <filter val="REEE-QEEQ"/>
-        <filter val="REEE-RSOSPQ"/>
-        <filter val="REEEE-RQQEO"/>
-        <filter val="REESQ-ASESEQ"/>
-        <filter val="REO-RSSEQ"/>
-        <filter val="REOP-S"/>
-        <filter val="REP-AEQ"/>
-        <filter val="REP-AQ"/>
-        <filter val="REPP-EEE"/>
-        <filter val="REQ-AP"/>
-        <filter val="REQ-ASQQ"/>
-        <filter val="REQ-QE"/>
-        <filter val="RER-RQ"/>
-        <filter val="RESEEQ-RSSS"/>
-        <filter val="RESSQ-AEO"/>
-        <filter val="ROE-QE"/>
-        <filter val="ROPQ-AEE"/>
-        <filter val="ROS-EE"/>
-        <filter val="ROS-RE"/>
-        <filter val="RQ-AE"/>
-        <filter val="RQ-AEE"/>
-        <filter val="RQ-AEEE"/>
-        <filter val="RQS-PEEPQ"/>
-        <filter val="RQS-RQSSE"/>
-        <filter val="RREQ-AE"/>
-        <filter val="RRQ-AE"/>
-        <filter val="RRRQP-AEAQ"/>
-        <filter val="RRSSSS-EEEE"/>
-        <filter val="RS-RSEQ"/>
-        <filter val="RSE-RRP"/>
-        <filter val="RSEEQ-AEE"/>
-        <filter val="RSES-ESEQE"/>
-        <filter val="RSQ-AEQ"/>
-        <filter val="RSS-OEEEQ"/>
-        <filter val="S-E"/>
-        <filter val="S-RE"/>
-        <filter val="S-REES"/>
-        <filter val="S-RREQ"/>
-        <filter val="SE-EE"/>
-        <filter val="SE-ES"/>
-        <filter val="SE-O"/>
-        <filter val="SE-PE"/>
-        <filter val="SE-RE"/>
-        <filter val="SE-REO"/>
-        <filter val="SE-RPP"/>
-        <filter val="SE-RREE"/>
-        <filter val="SE-SEEQ"/>
-        <filter val="SEE-ERE"/>
-        <filter val="SEE-REEO"/>
-        <filter val="SEE-SE"/>
-        <filter val="SEEE-EEEO"/>
-        <filter val="SEEEE-REEQ"/>
-        <filter val="SEP-REQ"/>
-        <filter val="SEQ-AESES"/>
-        <filter val="SEQQS-AS"/>
-        <filter val="SQ-AE"/>
-        <filter val="SQ-AEEE"/>
-        <filter val="SQ-EES"/>
-        <filter val="SQE-AEEE"/>
-        <filter val="SQQ-AASE"/>
-        <filter val="SS-EO"/>
-        <filter val="SS-EPE"/>
-        <filter val="SS-REPE"/>
-        <filter val="SSE-ROQ"/>
-        <filter val="SSESE-E"/>
-        <filter val="SSQ-AEQ"/>
-        <filter val="SSQS-AEQ"/>
-        <filter val="SSS-ESSP"/>
-        <filter val="SSSEE-EPP"/>
-        <filter val="SSSES-SSEEES"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AJ345">
       <sortCondition ref="A2:A345"/>
       <sortCondition ref="B2:B345"/>

</xml_diff>